<commit_message>
Changed +9V Net to +5V due to errors in LDO input voltage constraints
</commit_message>
<xml_diff>
--- a/mTouch_Test/mTouch_Test_bom_.xlsx
+++ b/mTouch_Test/mTouch_Test_bom_.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew Maatman\Documents\KiCad Projects\Projects\mTouch_Test_KiCAD\mTouch_Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8140008_{6D7849EE-794C-4BEA-962A-BF02143A6B8A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097BABF2-E679-427B-A3C9-044B31160E16}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7553"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mTouch_Test_bom_" sheetId="1" r:id="rId1"/>
@@ -412,8 +412,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -544,6 +544,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -890,10 +897,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1250,19 +1260,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.06640625" style="2"/>
+    <col min="2" max="2" width="9.08984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1297,11 +1307,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="213.75" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
@@ -1323,11 +1333,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C3" t="s">
@@ -1349,11 +1359,11 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C4" t="s">
@@ -1375,11 +1385,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C5" t="s">
@@ -1401,11 +1411,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C6" t="s">
@@ -1427,11 +1437,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C7" t="s">
@@ -1453,11 +1463,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C8" t="s">
@@ -1479,11 +1489,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C9" t="s">
@@ -1505,11 +1515,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C10" t="s">
@@ -1525,11 +1535,11 @@
         <v>603</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C11" t="s">
@@ -1545,11 +1555,11 @@
         <v>603</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C12" t="s">
@@ -1565,11 +1575,11 @@
         <v>603</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C13" t="s">
@@ -1585,11 +1595,11 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C14" t="s">
@@ -1599,11 +1609,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C15" t="s">
@@ -1619,11 +1629,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C16" t="s">
@@ -1639,11 +1649,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C17" t="s">
@@ -1659,11 +1669,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>66</v>
       </c>
       <c r="C18" t="s">
@@ -1679,11 +1689,11 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>69</v>
       </c>
       <c r="C19">
@@ -1705,11 +1715,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>72</v>
       </c>
       <c r="C20">
@@ -1731,11 +1741,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>74</v>
       </c>
       <c r="C21" t="s">
@@ -1757,11 +1767,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="114" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" ht="116" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C22" t="s">
@@ -1783,11 +1793,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C23">
@@ -1809,11 +1819,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C24">
@@ -1835,11 +1845,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>84</v>
       </c>
       <c r="C25" t="s">
@@ -1855,11 +1865,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>88</v>
       </c>
       <c r="C26" t="s">
@@ -1875,11 +1885,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="3" t="s">
         <v>92</v>
       </c>
       <c r="C27" t="s">
@@ -1895,11 +1905,11 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C28" t="s">
@@ -1915,11 +1925,11 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>99</v>
       </c>
       <c r="C29" t="s">
@@ -1935,11 +1945,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="3" t="s">
         <v>103</v>
       </c>
       <c r="C30" t="s">
@@ -1952,11 +1962,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="3" t="s">
         <v>107</v>
       </c>
       <c r="C31" t="s">
@@ -1972,11 +1982,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="3" t="s">
         <v>111</v>
       </c>
       <c r="C32" t="s">
@@ -1992,11 +2002,11 @@
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="3" t="s">
         <v>114</v>
       </c>
       <c r="C33" t="s">
@@ -2015,52 +2025,52 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>128</v>
       </c>

</xml_diff>